<commit_message>
Updated age groups for 2026 and 2025 VWF
</commit_message>
<xml_diff>
--- a/local/agegroups/2025-VWF.xlsx
+++ b/local/agegroups/2025-VWF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgonzalez/Projects/Misc/usaw-owlcms/local/agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7893CA-DEFD-7640-80F6-1D24AEE88722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F6134B-80C2-5F4A-8A48-53426F49C82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="500" windowWidth="39500" windowHeight="25100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="1880" windowWidth="39500" windowHeight="25100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AgeGroups" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="160">
   <si>
     <t>code</t>
   </si>
@@ -510,6 +510,12 @@
   </si>
   <si>
     <t>!UW30</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>ADAP U11</t>
   </si>
 </sst>
 </file>
@@ -852,11 +858,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y142"/>
+  <dimension ref="A1:Y146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -915,7 +919,7 @@
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
@@ -930,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G2" s="5" t="b">
         <f>TRUE()</f>
@@ -974,7 +978,7 @@
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>44</v>
@@ -986,10 +990,10 @@
         <v>6</v>
       </c>
       <c r="E3" s="4">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G3" s="5" t="b">
         <f>TRUE()</f>
@@ -998,7 +1002,9 @@
       <c r="I3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J3"/>
+      <c r="J3">
+        <v>36</v>
+      </c>
       <c r="K3">
         <v>40</v>
       </c>
@@ -1018,14 +1024,12 @@
         <v>63</v>
       </c>
       <c r="Q3" s="1">
-        <v>69</v>
-      </c>
-      <c r="R3" s="1">
-        <v>999</v>
-      </c>
-      <c r="S3" s="1"/>
+        <v>999</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3"/>
       <c r="T3" s="1"/>
-      <c r="U3"/>
+      <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -1033,7 +1037,7 @@
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>44</v>
@@ -1045,10 +1049,10 @@
         <v>6</v>
       </c>
       <c r="E4" s="4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" s="5" t="b">
         <f>TRUE()</f>
@@ -1058,7 +1062,9 @@
         <v>59</v>
       </c>
       <c r="J4"/>
-      <c r="K4"/>
+      <c r="K4">
+        <v>40</v>
+      </c>
       <c r="L4" s="1">
         <v>44</v>
       </c>
@@ -1078,13 +1084,11 @@
         <v>69</v>
       </c>
       <c r="R4" s="1">
-        <v>77</v>
-      </c>
-      <c r="S4" s="1">
-        <v>999</v>
-      </c>
+        <v>999</v>
+      </c>
+      <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
+      <c r="U4"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -1092,10 +1096,10 @@
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -1104,10 +1108,10 @@
         <v>6</v>
       </c>
       <c r="E5" s="4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F5" s="4">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G5" s="5" t="b">
         <f>TRUE()</f>
@@ -1116,12 +1120,8 @@
       <c r="I5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J5">
-        <v>36</v>
-      </c>
-      <c r="K5">
-        <v>40</v>
-      </c>
+      <c r="J5"/>
+      <c r="K5"/>
       <c r="L5" s="1">
         <v>44</v>
       </c>
@@ -1138,10 +1138,14 @@
         <v>63</v>
       </c>
       <c r="Q5" s="1">
-        <v>999</v>
-      </c>
-      <c r="R5" s="1"/>
-      <c r="S5"/>
+        <v>69</v>
+      </c>
+      <c r="R5" s="1">
+        <v>77</v>
+      </c>
+      <c r="S5" s="1">
+        <v>999</v>
+      </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
@@ -1151,7 +1155,7 @@
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>66</v>
@@ -1163,10 +1167,10 @@
         <v>6</v>
       </c>
       <c r="E6" s="4">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G6" s="5" t="b">
         <f>TRUE()</f>
@@ -1175,7 +1179,9 @@
       <c r="I6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J6"/>
+      <c r="J6">
+        <v>36</v>
+      </c>
       <c r="K6">
         <v>40</v>
       </c>
@@ -1195,14 +1201,12 @@
         <v>63</v>
       </c>
       <c r="Q6" s="1">
-        <v>69</v>
-      </c>
-      <c r="R6" s="1">
-        <v>999</v>
-      </c>
-      <c r="S6" s="1"/>
+        <v>999</v>
+      </c>
+      <c r="R6" s="1"/>
+      <c r="S6"/>
       <c r="T6" s="1"/>
-      <c r="U6"/>
+      <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
@@ -1210,7 +1214,7 @@
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>66</v>
@@ -1222,10 +1226,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="4">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F7" s="4">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G7" s="5" t="b">
         <f>TRUE()</f>
@@ -1234,8 +1238,12 @@
       <c r="I7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J7"/>
-      <c r="K7"/>
+      <c r="J7">
+        <v>36</v>
+      </c>
+      <c r="K7">
+        <v>40</v>
+      </c>
       <c r="L7" s="1">
         <v>44</v>
       </c>
@@ -1252,14 +1260,10 @@
         <v>63</v>
       </c>
       <c r="Q7" s="1">
-        <v>69</v>
-      </c>
-      <c r="R7" s="1">
-        <v>77</v>
-      </c>
-      <c r="S7" s="1">
-        <v>999</v>
-      </c>
+        <v>999</v>
+      </c>
+      <c r="R7" s="1"/>
+      <c r="S7"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
@@ -1269,10 +1273,10 @@
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1281,21 +1285,25 @@
         <v>6</v>
       </c>
       <c r="E8" s="4">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4">
         <v>15</v>
       </c>
-      <c r="F8" s="4">
-        <v>20</v>
-      </c>
       <c r="G8" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8" s="1"/>
+      <c r="K8">
+        <v>40</v>
+      </c>
+      <c r="L8" s="1">
+        <v>44</v>
+      </c>
       <c r="M8" s="1">
         <v>48</v>
       </c>
@@ -1312,15 +1320,11 @@
         <v>69</v>
       </c>
       <c r="R8" s="1">
-        <v>77</v>
-      </c>
-      <c r="S8" s="1">
-        <v>86</v>
-      </c>
-      <c r="T8" s="1">
-        <v>999</v>
-      </c>
-      <c r="U8" s="1"/>
+        <v>999</v>
+      </c>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -1328,10 +1332,10 @@
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -1340,21 +1344,23 @@
         <v>6</v>
       </c>
       <c r="E9" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G9" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J9"/>
       <c r="K9"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1">
+        <v>44</v>
+      </c>
       <c r="M9" s="1">
         <v>48</v>
       </c>
@@ -1374,35 +1380,33 @@
         <v>77</v>
       </c>
       <c r="S9" s="1">
-        <v>86</v>
-      </c>
-      <c r="T9" s="1">
-        <v>999</v>
-      </c>
+        <v>999</v>
+      </c>
+      <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F10" s="4">
-        <v>999</v>
+        <v>20</v>
       </c>
       <c r="G10" s="5" t="b">
         <f>TRUE()</f>
@@ -1444,12 +1448,12 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
@@ -1458,20 +1462,21 @@
         <v>6</v>
       </c>
       <c r="E11" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F11" s="4">
-        <v>999</v>
+        <v>20</v>
       </c>
       <c r="G11" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H11" s="6"/>
       <c r="I11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11" s="1"/>
       <c r="M11" s="1">
         <v>48</v>
       </c>
@@ -1502,31 +1507,31 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="4">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F12" s="4">
-        <v>39</v>
+        <v>999</v>
       </c>
       <c r="G12" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J12"/>
       <c r="K12"/>
@@ -1561,35 +1566,34 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="4">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F13" s="4">
-        <v>44</v>
+        <v>999</v>
       </c>
       <c r="G13" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H13" s="6"/>
       <c r="I13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="J13" s="1"/>
       <c r="M13" s="1">
         <v>48</v>
       </c>
@@ -1622,7 +1626,7 @@
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>46</v>
@@ -1634,10 +1638,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="4">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F14" s="4">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G14" s="5" t="b">
         <f>TRUE()</f>
@@ -1681,7 +1685,7 @@
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>46</v>
@@ -1693,10 +1697,10 @@
         <v>6</v>
       </c>
       <c r="E15" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F15" s="4">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G15" s="5" t="b">
         <f>TRUE()</f>
@@ -1740,7 +1744,7 @@
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>46</v>
@@ -1752,10 +1756,10 @@
         <v>6</v>
       </c>
       <c r="E16" s="4">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F16" s="4">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G16" s="5" t="b">
         <f>TRUE()</f>
@@ -1799,7 +1803,7 @@
     </row>
     <row r="17" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>46</v>
@@ -1811,10 +1815,10 @@
         <v>6</v>
       </c>
       <c r="E17" s="4">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F17" s="4">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G17" s="5" t="b">
         <f>TRUE()</f>
@@ -1858,7 +1862,7 @@
     </row>
     <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>46</v>
@@ -1870,10 +1874,10 @@
         <v>6</v>
       </c>
       <c r="E18" s="4">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F18" s="4">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="G18" s="5" t="b">
         <f>TRUE()</f>
@@ -1917,7 +1921,7 @@
     </row>
     <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>46</v>
@@ -1929,10 +1933,10 @@
         <v>6</v>
       </c>
       <c r="E19" s="4">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F19" s="4">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G19" s="5" t="b">
         <f>TRUE()</f>
@@ -1976,7 +1980,7 @@
     </row>
     <row r="20" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>46</v>
@@ -1988,10 +1992,10 @@
         <v>6</v>
       </c>
       <c r="E20" s="4">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F20" s="4">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G20" s="5" t="b">
         <f>TRUE()</f>
@@ -2035,7 +2039,7 @@
     </row>
     <row r="21" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>46</v>
@@ -2047,10 +2051,10 @@
         <v>6</v>
       </c>
       <c r="E21" s="4">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F21" s="4">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G21" s="5" t="b">
         <f>TRUE()</f>
@@ -2094,7 +2098,7 @@
     </row>
     <row r="22" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>46</v>
@@ -2106,10 +2110,10 @@
         <v>6</v>
       </c>
       <c r="E22" s="4">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F22" s="4">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G22" s="5" t="b">
         <f>TRUE()</f>
@@ -2153,7 +2157,7 @@
     </row>
     <row r="23" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>46</v>
@@ -2165,10 +2169,10 @@
         <v>6</v>
       </c>
       <c r="E23" s="4">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F23" s="4">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G23" s="5" t="b">
         <f>TRUE()</f>
@@ -2212,7 +2216,7 @@
     </row>
     <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>46</v>
@@ -2224,10 +2228,10 @@
         <v>6</v>
       </c>
       <c r="E24" s="4">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F24" s="4">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G24" s="5" t="b">
         <f>TRUE()</f>
@@ -2271,7 +2275,7 @@
     </row>
     <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>46</v>
@@ -2283,10 +2287,10 @@
         <v>6</v>
       </c>
       <c r="E25" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F25" s="4">
-        <v>999</v>
+        <v>94</v>
       </c>
       <c r="G25" s="5" t="b">
         <f>TRUE()</f>
@@ -2330,10 +2334,10 @@
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>11</v>
@@ -2342,10 +2346,10 @@
         <v>6</v>
       </c>
       <c r="E26" s="4">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="F26" s="4">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="G26" s="5" t="b">
         <f>TRUE()</f>
@@ -2389,10 +2393,10 @@
     </row>
     <row r="27" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
@@ -2401,10 +2405,10 @@
         <v>6</v>
       </c>
       <c r="E27" s="4">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="F27" s="4">
-        <v>44</v>
+        <v>999</v>
       </c>
       <c r="G27" s="5" t="b">
         <f>TRUE()</f>
@@ -2448,7 +2452,7 @@
     </row>
     <row r="28" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>67</v>
@@ -2460,10 +2464,10 @@
         <v>6</v>
       </c>
       <c r="E28" s="4">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F28" s="4">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G28" s="5" t="b">
         <f>TRUE()</f>
@@ -2507,7 +2511,7 @@
     </row>
     <row r="29" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>67</v>
@@ -2519,10 +2523,10 @@
         <v>6</v>
       </c>
       <c r="E29" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F29" s="4">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G29" s="5" t="b">
         <f>TRUE()</f>
@@ -2566,7 +2570,7 @@
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>67</v>
@@ -2578,10 +2582,10 @@
         <v>6</v>
       </c>
       <c r="E30" s="4">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F30" s="4">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G30" s="5" t="b">
         <f>TRUE()</f>
@@ -2625,7 +2629,7 @@
     </row>
     <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>67</v>
@@ -2637,10 +2641,10 @@
         <v>6</v>
       </c>
       <c r="E31" s="4">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F31" s="4">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G31" s="5" t="b">
         <f>TRUE()</f>
@@ -2684,7 +2688,7 @@
     </row>
     <row r="32" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>67</v>
@@ -2696,10 +2700,10 @@
         <v>6</v>
       </c>
       <c r="E32" s="4">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F32" s="4">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="G32" s="5" t="b">
         <f>TRUE()</f>
@@ -2743,7 +2747,7 @@
     </row>
     <row r="33" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>67</v>
@@ -2755,10 +2759,10 @@
         <v>6</v>
       </c>
       <c r="E33" s="4">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F33" s="4">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G33" s="5" t="b">
         <f>TRUE()</f>
@@ -2802,7 +2806,7 @@
     </row>
     <row r="34" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>67</v>
@@ -2814,10 +2818,10 @@
         <v>6</v>
       </c>
       <c r="E34" s="4">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F34" s="4">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G34" s="5" t="b">
         <f>TRUE()</f>
@@ -2861,7 +2865,7 @@
     </row>
     <row r="35" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>67</v>
@@ -2873,10 +2877,10 @@
         <v>6</v>
       </c>
       <c r="E35" s="4">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F35" s="4">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G35" s="5" t="b">
         <f>TRUE()</f>
@@ -2920,7 +2924,7 @@
     </row>
     <row r="36" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>67</v>
@@ -2932,10 +2936,10 @@
         <v>6</v>
       </c>
       <c r="E36" s="4">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F36" s="4">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G36" s="5" t="b">
         <f>TRUE()</f>
@@ -2979,7 +2983,7 @@
     </row>
     <row r="37" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>67</v>
@@ -2991,10 +2995,10 @@
         <v>6</v>
       </c>
       <c r="E37" s="4">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F37" s="4">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G37" s="5" t="b">
         <f>TRUE()</f>
@@ -3038,7 +3042,7 @@
     </row>
     <row r="38" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>67</v>
@@ -3050,10 +3054,10 @@
         <v>6</v>
       </c>
       <c r="E38" s="4">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F38" s="4">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G38" s="5" t="b">
         <f>TRUE()</f>
@@ -3097,7 +3101,7 @@
     </row>
     <row r="39" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>67</v>
@@ -3109,10 +3113,10 @@
         <v>6</v>
       </c>
       <c r="E39" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F39" s="4">
-        <v>999</v>
+        <v>94</v>
       </c>
       <c r="G39" s="5" t="b">
         <f>TRUE()</f>
@@ -3156,10 +3160,10 @@
     </row>
     <row r="40" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>11</v>
@@ -3168,10 +3172,10 @@
         <v>6</v>
       </c>
       <c r="E40" s="4">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="F40" s="4">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="G40" s="5" t="b">
         <f>TRUE()</f>
@@ -3215,10 +3219,10 @@
     </row>
     <row r="41" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>11</v>
@@ -3227,10 +3231,10 @@
         <v>6</v>
       </c>
       <c r="E41" s="4">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="F41" s="4">
-        <v>39</v>
+        <v>999</v>
       </c>
       <c r="G41" s="5" t="b">
         <f>TRUE()</f>
@@ -3274,7 +3278,7 @@
     </row>
     <row r="42" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>97</v>
+        <v>157</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>110</v>
@@ -3286,10 +3290,10 @@
         <v>6</v>
       </c>
       <c r="E42" s="4">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F42" s="4">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G42" s="5" t="b">
         <f>TRUE()</f>
@@ -3333,7 +3337,7 @@
     </row>
     <row r="43" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>110</v>
@@ -3345,10 +3349,10 @@
         <v>6</v>
       </c>
       <c r="E43" s="4">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F43" s="4">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G43" s="5" t="b">
         <f>TRUE()</f>
@@ -3392,7 +3396,7 @@
     </row>
     <row r="44" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>110</v>
@@ -3404,10 +3408,10 @@
         <v>6</v>
       </c>
       <c r="E44" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F44" s="4">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G44" s="5" t="b">
         <f>TRUE()</f>
@@ -3451,7 +3455,7 @@
     </row>
     <row r="45" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>110</v>
@@ -3463,10 +3467,10 @@
         <v>6</v>
       </c>
       <c r="E45" s="4">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F45" s="4">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G45" s="5" t="b">
         <f>TRUE()</f>
@@ -3510,7 +3514,7 @@
     </row>
     <row r="46" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>110</v>
@@ -3522,10 +3526,10 @@
         <v>6</v>
       </c>
       <c r="E46" s="4">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F46" s="4">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G46" s="5" t="b">
         <f>TRUE()</f>
@@ -3569,7 +3573,7 @@
     </row>
     <row r="47" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>110</v>
@@ -3581,10 +3585,10 @@
         <v>6</v>
       </c>
       <c r="E47" s="4">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F47" s="4">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="G47" s="5" t="b">
         <f>TRUE()</f>
@@ -3628,7 +3632,7 @@
     </row>
     <row r="48" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>110</v>
@@ -3640,10 +3644,10 @@
         <v>6</v>
       </c>
       <c r="E48" s="4">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F48" s="4">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G48" s="5" t="b">
         <f>TRUE()</f>
@@ -3687,7 +3691,7 @@
     </row>
     <row r="49" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>110</v>
@@ -3699,10 +3703,10 @@
         <v>6</v>
       </c>
       <c r="E49" s="4">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F49" s="4">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G49" s="5" t="b">
         <f>TRUE()</f>
@@ -3746,7 +3750,7 @@
     </row>
     <row r="50" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>110</v>
@@ -3758,10 +3762,10 @@
         <v>6</v>
       </c>
       <c r="E50" s="4">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F50" s="4">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G50" s="5" t="b">
         <f>TRUE()</f>
@@ -3805,7 +3809,7 @@
     </row>
     <row r="51" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>110</v>
@@ -3817,10 +3821,10 @@
         <v>6</v>
       </c>
       <c r="E51" s="4">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F51" s="4">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G51" s="5" t="b">
         <f>TRUE()</f>
@@ -3864,7 +3868,7 @@
     </row>
     <row r="52" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>110</v>
@@ -3876,10 +3880,10 @@
         <v>6</v>
       </c>
       <c r="E52" s="4">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F52" s="4">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G52" s="5" t="b">
         <f>TRUE()</f>
@@ -3923,7 +3927,7 @@
     </row>
     <row r="53" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>110</v>
@@ -3935,10 +3939,10 @@
         <v>6</v>
       </c>
       <c r="E53" s="4">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F53" s="4">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G53" s="5" t="b">
         <f>TRUE()</f>
@@ -3982,7 +3986,7 @@
     </row>
     <row r="54" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>110</v>
@@ -3994,10 +3998,10 @@
         <v>6</v>
       </c>
       <c r="E54" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F54" s="4">
-        <v>999</v>
+        <v>94</v>
       </c>
       <c r="G54" s="5" t="b">
         <f>TRUE()</f>
@@ -4041,10 +4045,10 @@
     </row>
     <row r="55" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>11</v>
@@ -4053,10 +4057,10 @@
         <v>6</v>
       </c>
       <c r="E55" s="4">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="F55" s="4">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="G55" s="5" t="b">
         <f>TRUE()</f>
@@ -4100,10 +4104,10 @@
     </row>
     <row r="56" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>11</v>
@@ -4112,10 +4116,10 @@
         <v>6</v>
       </c>
       <c r="E56" s="4">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="F56" s="4">
-        <v>39</v>
+        <v>999</v>
       </c>
       <c r="G56" s="5" t="b">
         <f>TRUE()</f>
@@ -4159,7 +4163,7 @@
     </row>
     <row r="57" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>125</v>
@@ -4171,10 +4175,10 @@
         <v>6</v>
       </c>
       <c r="E57" s="4">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F57" s="4">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G57" s="5" t="b">
         <f>TRUE()</f>
@@ -4218,7 +4222,7 @@
     </row>
     <row r="58" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>125</v>
@@ -4230,10 +4234,10 @@
         <v>6</v>
       </c>
       <c r="E58" s="4">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F58" s="4">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G58" s="5" t="b">
         <f>TRUE()</f>
@@ -4277,7 +4281,7 @@
     </row>
     <row r="59" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>125</v>
@@ -4289,10 +4293,10 @@
         <v>6</v>
       </c>
       <c r="E59" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F59" s="4">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G59" s="5" t="b">
         <f>TRUE()</f>
@@ -4336,7 +4340,7 @@
     </row>
     <row r="60" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>125</v>
@@ -4348,10 +4352,10 @@
         <v>6</v>
       </c>
       <c r="E60" s="4">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F60" s="4">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G60" s="5" t="b">
         <f>TRUE()</f>
@@ -4395,7 +4399,7 @@
     </row>
     <row r="61" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>125</v>
@@ -4407,10 +4411,10 @@
         <v>6</v>
       </c>
       <c r="E61" s="4">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F61" s="4">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G61" s="5" t="b">
         <f>TRUE()</f>
@@ -4454,7 +4458,7 @@
     </row>
     <row r="62" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>125</v>
@@ -4466,10 +4470,10 @@
         <v>6</v>
       </c>
       <c r="E62" s="4">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F62" s="4">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="G62" s="5" t="b">
         <f>TRUE()</f>
@@ -4513,7 +4517,7 @@
     </row>
     <row r="63" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>125</v>
@@ -4525,10 +4529,10 @@
         <v>6</v>
       </c>
       <c r="E63" s="4">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F63" s="4">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G63" s="5" t="b">
         <f>TRUE()</f>
@@ -4572,7 +4576,7 @@
     </row>
     <row r="64" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>125</v>
@@ -4584,10 +4588,10 @@
         <v>6</v>
       </c>
       <c r="E64" s="4">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F64" s="4">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G64" s="5" t="b">
         <f>TRUE()</f>
@@ -4631,7 +4635,7 @@
     </row>
     <row r="65" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>125</v>
@@ -4643,10 +4647,10 @@
         <v>6</v>
       </c>
       <c r="E65" s="4">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F65" s="4">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G65" s="5" t="b">
         <f>TRUE()</f>
@@ -4690,7 +4694,7 @@
     </row>
     <row r="66" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>125</v>
@@ -4702,10 +4706,10 @@
         <v>6</v>
       </c>
       <c r="E66" s="4">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F66" s="4">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G66" s="5" t="b">
         <f>TRUE()</f>
@@ -4749,7 +4753,7 @@
     </row>
     <row r="67" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>125</v>
@@ -4761,10 +4765,10 @@
         <v>6</v>
       </c>
       <c r="E67" s="4">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F67" s="4">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G67" s="5" t="b">
         <f>TRUE()</f>
@@ -4808,7 +4812,7 @@
     </row>
     <row r="68" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>125</v>
@@ -4820,10 +4824,10 @@
         <v>6</v>
       </c>
       <c r="E68" s="4">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F68" s="4">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G68" s="5" t="b">
         <f>TRUE()</f>
@@ -4867,7 +4871,7 @@
     </row>
     <row r="69" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>125</v>
@@ -4879,10 +4883,10 @@
         <v>6</v>
       </c>
       <c r="E69" s="4">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F69" s="4">
-        <v>999</v>
+        <v>94</v>
       </c>
       <c r="G69" s="5" t="b">
         <f>TRUE()</f>
@@ -4924,43 +4928,56 @@
       <c r="X69" s="1"/>
       <c r="Y69" s="1"/>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>47</v>
+        <v>123</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E70" s="4">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="F70" s="4">
-        <v>999</v>
+        <v>99</v>
       </c>
       <c r="G70" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H70" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="I70" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="J70"/>
+      <c r="K70"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1">
+        <v>48</v>
+      </c>
+      <c r="N70" s="1">
+        <v>53</v>
+      </c>
+      <c r="O70" s="1">
+        <v>58</v>
+      </c>
+      <c r="P70" s="1">
+        <v>63</v>
+      </c>
+      <c r="Q70" s="1">
+        <v>69</v>
+      </c>
+      <c r="R70" s="1">
+        <v>77</v>
+      </c>
+      <c r="S70" s="1">
+        <v>86</v>
+      </c>
       <c r="T70" s="1">
         <v>999</v>
       </c>
@@ -4970,12 +4987,12 @@
       <c r="X70" s="1"/>
       <c r="Y70" s="1"/>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>11</v>
@@ -4984,7 +5001,7 @@
         <v>6</v>
       </c>
       <c r="E71" s="4">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="F71" s="4">
         <v>999</v>
@@ -4993,20 +5010,33 @@
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H71" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="I71" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
-      <c r="S71" s="1"/>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1">
+        <v>48</v>
+      </c>
+      <c r="N71" s="1">
+        <v>53</v>
+      </c>
+      <c r="O71" s="1">
+        <v>58</v>
+      </c>
+      <c r="P71" s="1">
+        <v>63</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>69</v>
+      </c>
+      <c r="R71" s="1">
+        <v>77</v>
+      </c>
+      <c r="S71" s="1">
+        <v>86</v>
+      </c>
       <c r="T71" s="1">
         <v>999</v>
       </c>
@@ -5018,123 +5048,99 @@
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E72" s="4">
         <v>0</v>
       </c>
       <c r="F72" s="4">
-        <v>13</v>
+        <v>999</v>
       </c>
       <c r="G72" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H72" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="I72" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J72" s="1">
-        <v>40</v>
-      </c>
-      <c r="K72">
-        <v>44</v>
-      </c>
-      <c r="L72">
-        <v>48</v>
-      </c>
-      <c r="M72" s="1">
-        <v>52</v>
-      </c>
-      <c r="N72" s="1">
-        <v>56</v>
-      </c>
-      <c r="O72" s="1">
-        <v>60</v>
-      </c>
-      <c r="P72" s="1">
-        <v>65</v>
-      </c>
-      <c r="Q72" s="1">
-        <v>999</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="J72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
-      <c r="T72" s="1"/>
+      <c r="T72" s="1">
+        <v>999</v>
+      </c>
       <c r="U72" s="1"/>
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
       <c r="X72" s="1"/>
+      <c r="Y72" s="1"/>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E73" s="4">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="F73" s="4">
-        <v>15</v>
+        <v>999</v>
       </c>
       <c r="G73" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H73" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="I73" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J73" s="1"/>
-      <c r="K73"/>
-      <c r="L73">
-        <v>48</v>
-      </c>
-      <c r="M73" s="1">
-        <v>52</v>
-      </c>
-      <c r="N73" s="1">
-        <v>56</v>
-      </c>
-      <c r="O73" s="1">
-        <v>60</v>
-      </c>
-      <c r="P73" s="1">
-        <v>65</v>
-      </c>
-      <c r="Q73" s="1">
-        <v>71</v>
-      </c>
-      <c r="R73" s="1">
-        <v>79</v>
-      </c>
-      <c r="S73" s="1">
-        <v>999</v>
-      </c>
-      <c r="T73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1">
+        <v>999</v>
+      </c>
       <c r="U73" s="1"/>
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
       <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>9</v>
+        <v>158</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>44</v>
@@ -5146,10 +5152,10 @@
         <v>28</v>
       </c>
       <c r="E74" s="4">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F74" s="4">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G74" s="5" t="b">
         <f>TRUE()</f>
@@ -5158,9 +5164,18 @@
       <c r="I74" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J74"/>
-      <c r="K74"/>
-      <c r="L74" s="1"/>
+      <c r="J74" s="1">
+        <v>40</v>
+      </c>
+      <c r="K74">
+        <v>44</v>
+      </c>
+      <c r="L74">
+        <v>48</v>
+      </c>
+      <c r="M74" s="1">
+        <v>52</v>
+      </c>
       <c r="N74" s="1">
         <v>56</v>
       </c>
@@ -5171,30 +5186,22 @@
         <v>65</v>
       </c>
       <c r="Q74" s="1">
-        <v>71</v>
-      </c>
-      <c r="R74" s="1">
-        <v>79</v>
-      </c>
-      <c r="S74" s="1">
-        <v>88</v>
-      </c>
-      <c r="T74" s="1">
-        <v>94</v>
-      </c>
-      <c r="U74" s="1">
-        <v>999</v>
-      </c>
+        <v>999</v>
+      </c>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
       <c r="X74" s="1"/>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>5</v>
@@ -5249,10 +5256,10 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>5</v>
@@ -5307,10 +5314,10 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>5</v>
@@ -5364,10 +5371,10 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>25</v>
+        <v>159</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>5</v>
@@ -5376,22 +5383,33 @@
         <v>28</v>
       </c>
       <c r="E78" s="4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F78" s="4">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G78" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J78"/>
-      <c r="K78"/>
-      <c r="L78" s="1"/>
-      <c r="N78" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="J78" s="1">
+        <v>40</v>
+      </c>
+      <c r="K78">
+        <v>44</v>
+      </c>
+      <c r="L78">
+        <v>48</v>
+      </c>
+      <c r="M78" s="1">
+        <v>52</v>
+      </c>
+      <c r="N78" s="1">
+        <v>56</v>
+      </c>
       <c r="O78" s="1">
         <v>60</v>
       </c>
@@ -5399,32 +5417,22 @@
         <v>65</v>
       </c>
       <c r="Q78" s="1">
-        <v>71</v>
-      </c>
-      <c r="R78" s="1">
-        <v>79</v>
-      </c>
-      <c r="S78" s="1">
-        <v>88</v>
-      </c>
-      <c r="T78" s="1">
-        <v>94</v>
-      </c>
-      <c r="U78" s="1">
-        <v>110</v>
-      </c>
-      <c r="V78" s="1">
-        <v>999</v>
-      </c>
+        <v>999</v>
+      </c>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
       <c r="W78" s="1"/>
       <c r="X78" s="1"/>
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>5</v>
@@ -5433,22 +5441,33 @@
         <v>28</v>
       </c>
       <c r="E79" s="4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F79" s="4">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G79" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J79"/>
-      <c r="K79"/>
-      <c r="L79" s="1"/>
-      <c r="N79" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="J79" s="1">
+        <v>40</v>
+      </c>
+      <c r="K79">
+        <v>44</v>
+      </c>
+      <c r="L79">
+        <v>48</v>
+      </c>
+      <c r="M79" s="1">
+        <v>52</v>
+      </c>
+      <c r="N79" s="1">
+        <v>56</v>
+      </c>
       <c r="O79" s="1">
         <v>60</v>
       </c>
@@ -5456,56 +5475,53 @@
         <v>65</v>
       </c>
       <c r="Q79" s="1">
-        <v>71</v>
-      </c>
-      <c r="R79" s="1">
-        <v>79</v>
-      </c>
-      <c r="S79" s="1">
-        <v>88</v>
-      </c>
-      <c r="T79" s="1">
-        <v>94</v>
-      </c>
-      <c r="U79" s="1">
-        <v>110</v>
-      </c>
-      <c r="V79" s="1">
-        <v>999</v>
-      </c>
+        <v>999</v>
+      </c>
+      <c r="R79" s="1"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="1"/>
+      <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E80" s="4">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F80" s="4">
-        <v>999</v>
+        <v>15</v>
       </c>
       <c r="G80" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J80"/>
+        <v>59</v>
+      </c>
+      <c r="J80" s="1"/>
       <c r="K80"/>
-      <c r="L80" s="1"/>
-      <c r="N80" s="1"/>
+      <c r="L80">
+        <v>48</v>
+      </c>
+      <c r="M80" s="1">
+        <v>52</v>
+      </c>
+      <c r="N80" s="1">
+        <v>56</v>
+      </c>
       <c r="O80" s="1">
         <v>60</v>
       </c>
@@ -5519,26 +5535,20 @@
         <v>79</v>
       </c>
       <c r="S80" s="1">
-        <v>88</v>
-      </c>
-      <c r="T80" s="1">
-        <v>94</v>
-      </c>
-      <c r="U80" s="1">
-        <v>110</v>
-      </c>
-      <c r="V80" s="1">
-        <v>999</v>
-      </c>
+        <v>999</v>
+      </c>
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
       <c r="W80" s="1"/>
       <c r="X80" s="1"/>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>5</v>
@@ -5547,23 +5557,24 @@
         <v>28</v>
       </c>
       <c r="E81" s="4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F81" s="4">
-        <v>999</v>
+        <v>17</v>
       </c>
       <c r="G81" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H81" s="6"/>
       <c r="I81" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="J81"/>
+      <c r="K81"/>
       <c r="L81" s="1"/>
-      <c r="N81" s="1"/>
+      <c r="N81" s="1">
+        <v>56</v>
+      </c>
       <c r="O81" s="1">
         <v>60</v>
       </c>
@@ -5583,39 +5594,37 @@
         <v>94</v>
       </c>
       <c r="U81" s="1">
-        <v>110</v>
-      </c>
-      <c r="V81" s="1">
-        <v>999</v>
-      </c>
+        <v>999</v>
+      </c>
+      <c r="V81" s="1"/>
       <c r="W81" s="1"/>
       <c r="X81" s="1"/>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E82" s="4">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F82" s="4">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G82" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J82"/>
       <c r="K82"/>
@@ -5650,29 +5659,29 @@
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E83" s="4">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F83" s="4">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="G83" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J83"/>
       <c r="K83"/>
@@ -5707,29 +5716,29 @@
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E84" s="4">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F84" s="4">
-        <v>49</v>
+        <v>999</v>
       </c>
       <c r="G84" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J84"/>
       <c r="K84"/>
@@ -5764,32 +5773,33 @@
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E85" s="4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F85" s="4">
-        <v>54</v>
+        <v>999</v>
       </c>
       <c r="G85" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
+      <c r="H85" s="6"/>
       <c r="I85" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J85"/>
-      <c r="K85"/>
+        <v>57</v>
+      </c>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
       <c r="L85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1">
@@ -5821,7 +5831,7 @@
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>46</v>
@@ -5833,10 +5843,10 @@
         <v>28</v>
       </c>
       <c r="E86" s="4">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="F86" s="4">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="G86" s="5" t="b">
         <f>TRUE()</f>
@@ -5878,7 +5888,7 @@
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>46</v>
@@ -5890,10 +5900,10 @@
         <v>28</v>
       </c>
       <c r="E87" s="4">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F87" s="4">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="G87" s="5" t="b">
         <f>TRUE()</f>
@@ -5935,7 +5945,7 @@
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>46</v>
@@ -5947,10 +5957,10 @@
         <v>28</v>
       </c>
       <c r="E88" s="4">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F88" s="4">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="G88" s="5" t="b">
         <f>TRUE()</f>
@@ -5992,7 +6002,7 @@
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>46</v>
@@ -6004,10 +6014,10 @@
         <v>28</v>
       </c>
       <c r="E89" s="4">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F89" s="4">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="G89" s="5" t="b">
         <f>TRUE()</f>
@@ -6049,7 +6059,7 @@
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>46</v>
@@ -6061,10 +6071,10 @@
         <v>28</v>
       </c>
       <c r="E90" s="4">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="F90" s="4">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="G90" s="5" t="b">
         <f>TRUE()</f>
@@ -6105,8 +6115,8 @@
       <c r="X90" s="1"/>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A91" s="7" t="s">
-        <v>38</v>
+      <c r="A91" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>46</v>
@@ -6118,10 +6128,10 @@
         <v>28</v>
       </c>
       <c r="E91" s="4">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F91" s="4">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="G91" s="5" t="b">
         <f>TRUE()</f>
@@ -6162,8 +6172,8 @@
       <c r="X91" s="1"/>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A92" s="7" t="s">
-        <v>39</v>
+      <c r="A92" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>46</v>
@@ -6175,10 +6185,10 @@
         <v>28</v>
       </c>
       <c r="E92" s="4">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F92" s="4">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="G92" s="5" t="b">
         <f>TRUE()</f>
@@ -6219,8 +6229,8 @@
       <c r="X92" s="1"/>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A93" s="7" t="s">
-        <v>40</v>
+      <c r="A93" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>46</v>
@@ -6232,10 +6242,10 @@
         <v>28</v>
       </c>
       <c r="E93" s="4">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F93" s="4">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="G93" s="5" t="b">
         <f>TRUE()</f>
@@ -6276,8 +6286,8 @@
       <c r="X93" s="1"/>
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A94" s="7" t="s">
-        <v>41</v>
+      <c r="A94" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>46</v>
@@ -6289,10 +6299,10 @@
         <v>28</v>
       </c>
       <c r="E94" s="4">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="F94" s="4">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="G94" s="5" t="b">
         <f>TRUE()</f>
@@ -6334,7 +6344,7 @@
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>46</v>
@@ -6346,10 +6356,10 @@
         <v>28</v>
       </c>
       <c r="E95" s="4">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F95" s="4">
-        <v>999</v>
+        <v>84</v>
       </c>
       <c r="G95" s="5" t="b">
         <f>TRUE()</f>
@@ -6390,11 +6400,11 @@
       <c r="X95" s="1"/>
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>82</v>
+      <c r="A96" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>11</v>
@@ -6403,10 +6413,10 @@
         <v>28</v>
       </c>
       <c r="E96" s="4">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="F96" s="4">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="G96" s="5" t="b">
         <f>TRUE()</f>
@@ -6447,11 +6457,11 @@
       <c r="X96" s="1"/>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
-        <v>83</v>
+      <c r="A97" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>11</v>
@@ -6460,10 +6470,10 @@
         <v>28</v>
       </c>
       <c r="E97" s="4">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="F97" s="4">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="G97" s="5" t="b">
         <f>TRUE()</f>
@@ -6504,11 +6514,11 @@
       <c r="X97" s="1"/>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>84</v>
+      <c r="A98" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>11</v>
@@ -6517,10 +6527,10 @@
         <v>28</v>
       </c>
       <c r="E98" s="4">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="F98" s="4">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="G98" s="5" t="b">
         <f>TRUE()</f>
@@ -6561,11 +6571,11 @@
       <c r="X98" s="1"/>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>85</v>
+      <c r="A99" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>11</v>
@@ -6574,10 +6584,10 @@
         <v>28</v>
       </c>
       <c r="E99" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F99" s="4">
-        <v>54</v>
+        <v>999</v>
       </c>
       <c r="G99" s="5" t="b">
         <f>TRUE()</f>
@@ -6619,7 +6629,7 @@
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>67</v>
@@ -6631,10 +6641,10 @@
         <v>28</v>
       </c>
       <c r="E100" s="4">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="F100" s="4">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="G100" s="5" t="b">
         <f>TRUE()</f>
@@ -6676,7 +6686,7 @@
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>67</v>
@@ -6688,10 +6698,10 @@
         <v>28</v>
       </c>
       <c r="E101" s="4">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F101" s="4">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="G101" s="5" t="b">
         <f>TRUE()</f>
@@ -6733,7 +6743,7 @@
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>67</v>
@@ -6745,10 +6755,10 @@
         <v>28</v>
       </c>
       <c r="E102" s="4">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F102" s="4">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="G102" s="5" t="b">
         <f>TRUE()</f>
@@ -6790,7 +6800,7 @@
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>67</v>
@@ -6802,10 +6812,10 @@
         <v>28</v>
       </c>
       <c r="E103" s="4">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F103" s="4">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="G103" s="5" t="b">
         <f>TRUE()</f>
@@ -6847,7 +6857,7 @@
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>67</v>
@@ -6859,10 +6869,10 @@
         <v>28</v>
       </c>
       <c r="E104" s="4">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="F104" s="4">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="G104" s="5" t="b">
         <f>TRUE()</f>
@@ -6903,8 +6913,8 @@
       <c r="X104" s="1"/>
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A105" s="7" t="s">
-        <v>91</v>
+      <c r="A105" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>67</v>
@@ -6916,10 +6926,10 @@
         <v>28</v>
       </c>
       <c r="E105" s="4">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F105" s="4">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="G105" s="5" t="b">
         <f>TRUE()</f>
@@ -6960,8 +6970,8 @@
       <c r="X105" s="1"/>
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A106" s="7" t="s">
-        <v>92</v>
+      <c r="A106" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>67</v>
@@ -6973,10 +6983,10 @@
         <v>28</v>
       </c>
       <c r="E106" s="4">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F106" s="4">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="G106" s="5" t="b">
         <f>TRUE()</f>
@@ -7017,8 +7027,8 @@
       <c r="X106" s="1"/>
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A107" s="7" t="s">
-        <v>93</v>
+      <c r="A107" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>67</v>
@@ -7030,10 +7040,10 @@
         <v>28</v>
       </c>
       <c r="E107" s="4">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F107" s="4">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="G107" s="5" t="b">
         <f>TRUE()</f>
@@ -7074,8 +7084,8 @@
       <c r="X107" s="1"/>
     </row>
     <row r="108" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A108" s="7" t="s">
-        <v>94</v>
+      <c r="A108" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>67</v>
@@ -7087,10 +7097,10 @@
         <v>28</v>
       </c>
       <c r="E108" s="4">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="F108" s="4">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="G108" s="5" t="b">
         <f>TRUE()</f>
@@ -7132,7 +7142,7 @@
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>67</v>
@@ -7144,10 +7154,10 @@
         <v>28</v>
       </c>
       <c r="E109" s="4">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F109" s="4">
-        <v>999</v>
+        <v>84</v>
       </c>
       <c r="G109" s="5" t="b">
         <f>TRUE()</f>
@@ -7188,11 +7198,11 @@
       <c r="X109" s="1"/>
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
-        <v>155</v>
+      <c r="A110" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>11</v>
@@ -7201,10 +7211,10 @@
         <v>28</v>
       </c>
       <c r="E110" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="F110" s="4">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="G110" s="5" t="b">
         <f>TRUE()</f>
@@ -7245,11 +7255,11 @@
       <c r="X110" s="1"/>
     </row>
     <row r="111" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>126</v>
+      <c r="A111" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>11</v>
@@ -7258,10 +7268,10 @@
         <v>28</v>
       </c>
       <c r="E111" s="4">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="F111" s="4">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="G111" s="5" t="b">
         <f>TRUE()</f>
@@ -7302,11 +7312,11 @@
       <c r="X111" s="1"/>
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
-        <v>127</v>
+      <c r="A112" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>11</v>
@@ -7315,10 +7325,10 @@
         <v>28</v>
       </c>
       <c r="E112" s="4">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="F112" s="4">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="G112" s="5" t="b">
         <f>TRUE()</f>
@@ -7359,11 +7369,11 @@
       <c r="X112" s="1"/>
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>128</v>
+      <c r="A113" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>11</v>
@@ -7372,10 +7382,10 @@
         <v>28</v>
       </c>
       <c r="E113" s="4">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="F113" s="4">
-        <v>49</v>
+        <v>999</v>
       </c>
       <c r="G113" s="5" t="b">
         <f>TRUE()</f>
@@ -7417,7 +7427,7 @@
     </row>
     <row r="114" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>110</v>
@@ -7429,10 +7439,10 @@
         <v>28</v>
       </c>
       <c r="E114" s="4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F114" s="4">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="G114" s="5" t="b">
         <f>TRUE()</f>
@@ -7474,7 +7484,7 @@
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>110</v>
@@ -7486,10 +7496,10 @@
         <v>28</v>
       </c>
       <c r="E115" s="4">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="F115" s="4">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="G115" s="5" t="b">
         <f>TRUE()</f>
@@ -7531,7 +7541,7 @@
     </row>
     <row r="116" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>110</v>
@@ -7543,10 +7553,10 @@
         <v>28</v>
       </c>
       <c r="E116" s="4">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F116" s="4">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="G116" s="5" t="b">
         <f>TRUE()</f>
@@ -7588,7 +7598,7 @@
     </row>
     <row r="117" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>110</v>
@@ -7600,10 +7610,10 @@
         <v>28</v>
       </c>
       <c r="E117" s="4">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F117" s="4">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="G117" s="5" t="b">
         <f>TRUE()</f>
@@ -7645,7 +7655,7 @@
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>110</v>
@@ -7657,10 +7667,10 @@
         <v>28</v>
       </c>
       <c r="E118" s="4">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F118" s="4">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="G118" s="5" t="b">
         <f>TRUE()</f>
@@ -7702,7 +7712,7 @@
     </row>
     <row r="119" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>110</v>
@@ -7714,10 +7724,10 @@
         <v>28</v>
       </c>
       <c r="E119" s="4">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="F119" s="4">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="G119" s="5" t="b">
         <f>TRUE()</f>
@@ -7759,7 +7769,7 @@
     </row>
     <row r="120" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>110</v>
@@ -7771,10 +7781,10 @@
         <v>28</v>
       </c>
       <c r="E120" s="4">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F120" s="4">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="G120" s="5" t="b">
         <f>TRUE()</f>
@@ -7816,7 +7826,7 @@
     </row>
     <row r="121" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>110</v>
@@ -7828,10 +7838,10 @@
         <v>28</v>
       </c>
       <c r="E121" s="4">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F121" s="4">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="G121" s="5" t="b">
         <f>TRUE()</f>
@@ -7873,7 +7883,7 @@
     </row>
     <row r="122" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>110</v>
@@ -7885,10 +7895,10 @@
         <v>28</v>
       </c>
       <c r="E122" s="4">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F122" s="4">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="G122" s="5" t="b">
         <f>TRUE()</f>
@@ -7930,7 +7940,7 @@
     </row>
     <row r="123" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>110</v>
@@ -7942,10 +7952,10 @@
         <v>28</v>
       </c>
       <c r="E123" s="4">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="F123" s="4">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="G123" s="5" t="b">
         <f>TRUE()</f>
@@ -7987,7 +7997,7 @@
     </row>
     <row r="124" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>110</v>
@@ -7999,10 +8009,10 @@
         <v>28</v>
       </c>
       <c r="E124" s="4">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F124" s="4">
-        <v>999</v>
+        <v>84</v>
       </c>
       <c r="G124" s="5" t="b">
         <f>TRUE()</f>
@@ -8044,10 +8054,10 @@
     </row>
     <row r="125" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>11</v>
@@ -8056,10 +8066,10 @@
         <v>28</v>
       </c>
       <c r="E125" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="F125" s="4">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="G125" s="5" t="b">
         <f>TRUE()</f>
@@ -8101,10 +8111,10 @@
     </row>
     <row r="126" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>11</v>
@@ -8113,10 +8123,10 @@
         <v>28</v>
       </c>
       <c r="E126" s="4">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="F126" s="4">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="G126" s="5" t="b">
         <f>TRUE()</f>
@@ -8158,10 +8168,10 @@
     </row>
     <row r="127" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>11</v>
@@ -8170,10 +8180,10 @@
         <v>28</v>
       </c>
       <c r="E127" s="4">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="F127" s="4">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="G127" s="5" t="b">
         <f>TRUE()</f>
@@ -8215,10 +8225,10 @@
     </row>
     <row r="128" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>11</v>
@@ -8227,10 +8237,10 @@
         <v>28</v>
       </c>
       <c r="E128" s="4">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="F128" s="4">
-        <v>49</v>
+        <v>999</v>
       </c>
       <c r="G128" s="5" t="b">
         <f>TRUE()</f>
@@ -8272,7 +8282,7 @@
     </row>
     <row r="129" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>125</v>
@@ -8284,10 +8294,10 @@
         <v>28</v>
       </c>
       <c r="E129" s="4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F129" s="4">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="G129" s="5" t="b">
         <f>TRUE()</f>
@@ -8329,7 +8339,7 @@
     </row>
     <row r="130" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>125</v>
@@ -8341,10 +8351,10 @@
         <v>28</v>
       </c>
       <c r="E130" s="4">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="F130" s="4">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="G130" s="5" t="b">
         <f>TRUE()</f>
@@ -8386,7 +8396,7 @@
     </row>
     <row r="131" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>125</v>
@@ -8398,10 +8408,10 @@
         <v>28</v>
       </c>
       <c r="E131" s="4">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F131" s="4">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="G131" s="5" t="b">
         <f>TRUE()</f>
@@ -8443,7 +8453,7 @@
     </row>
     <row r="132" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>125</v>
@@ -8455,10 +8465,10 @@
         <v>28</v>
       </c>
       <c r="E132" s="4">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F132" s="4">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="G132" s="5" t="b">
         <f>TRUE()</f>
@@ -8500,7 +8510,7 @@
     </row>
     <row r="133" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>125</v>
@@ -8512,10 +8522,10 @@
         <v>28</v>
       </c>
       <c r="E133" s="4">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F133" s="4">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="G133" s="5" t="b">
         <f>TRUE()</f>
@@ -8557,7 +8567,7 @@
     </row>
     <row r="134" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>125</v>
@@ -8569,10 +8579,10 @@
         <v>28</v>
       </c>
       <c r="E134" s="4">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="F134" s="4">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="G134" s="5" t="b">
         <f>TRUE()</f>
@@ -8614,7 +8624,7 @@
     </row>
     <row r="135" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>125</v>
@@ -8626,10 +8636,10 @@
         <v>28</v>
       </c>
       <c r="E135" s="4">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F135" s="4">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="G135" s="5" t="b">
         <f>TRUE()</f>
@@ -8671,7 +8681,7 @@
     </row>
     <row r="136" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>125</v>
@@ -8683,10 +8693,10 @@
         <v>28</v>
       </c>
       <c r="E136" s="4">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F136" s="4">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="G136" s="5" t="b">
         <f>TRUE()</f>
@@ -8728,7 +8738,7 @@
     </row>
     <row r="137" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>125</v>
@@ -8740,10 +8750,10 @@
         <v>28</v>
       </c>
       <c r="E137" s="4">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F137" s="4">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="G137" s="5" t="b">
         <f>TRUE()</f>
@@ -8785,7 +8795,7 @@
     </row>
     <row r="138" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>125</v>
@@ -8797,10 +8807,10 @@
         <v>28</v>
       </c>
       <c r="E138" s="4">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="F138" s="4">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="G138" s="5" t="b">
         <f>TRUE()</f>
@@ -8842,7 +8852,7 @@
     </row>
     <row r="139" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>125</v>
@@ -8854,10 +8864,10 @@
         <v>28</v>
       </c>
       <c r="E139" s="4">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F139" s="4">
-        <v>999</v>
+        <v>84</v>
       </c>
       <c r="G139" s="5" t="b">
         <f>TRUE()</f>
@@ -8899,44 +8909,55 @@
     </row>
     <row r="140" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>47</v>
+        <v>150</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E140" s="4">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F140" s="4">
-        <v>999</v>
+        <v>89</v>
       </c>
       <c r="G140" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H140" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="I140" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J140" s="1"/>
-      <c r="K140" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="J140"/>
+      <c r="K140"/>
       <c r="L140" s="1"/>
       <c r="N140" s="1"/>
-      <c r="O140" s="1"/>
-      <c r="P140" s="1"/>
-      <c r="Q140" s="1"/>
-      <c r="R140" s="1"/>
-      <c r="S140" s="1"/>
-      <c r="T140" s="1"/>
-      <c r="U140" s="1"/>
+      <c r="O140" s="1">
+        <v>60</v>
+      </c>
+      <c r="P140" s="1">
+        <v>65</v>
+      </c>
+      <c r="Q140" s="1">
+        <v>71</v>
+      </c>
+      <c r="R140" s="1">
+        <v>79</v>
+      </c>
+      <c r="S140" s="1">
+        <v>88</v>
+      </c>
+      <c r="T140" s="1">
+        <v>94</v>
+      </c>
+      <c r="U140" s="1">
+        <v>110</v>
+      </c>
       <c r="V140" s="1">
         <v>999</v>
       </c>
@@ -8945,10 +8966,10 @@
     </row>
     <row r="141" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>52</v>
+        <v>151</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>11</v>
@@ -8957,32 +8978,43 @@
         <v>28</v>
       </c>
       <c r="E141" s="4">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="F141" s="4">
-        <v>999</v>
+        <v>99</v>
       </c>
       <c r="G141" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H141" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="I141" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J141" s="1"/>
-      <c r="K141" s="1"/>
+      <c r="J141"/>
+      <c r="K141"/>
       <c r="L141" s="1"/>
       <c r="N141" s="1"/>
-      <c r="O141" s="1"/>
-      <c r="P141" s="1"/>
-      <c r="Q141" s="1"/>
-      <c r="R141" s="1"/>
-      <c r="S141" s="1"/>
-      <c r="T141" s="1"/>
-      <c r="U141" s="1"/>
+      <c r="O141" s="1">
+        <v>60</v>
+      </c>
+      <c r="P141" s="1">
+        <v>65</v>
+      </c>
+      <c r="Q141" s="1">
+        <v>71</v>
+      </c>
+      <c r="R141" s="1">
+        <v>79</v>
+      </c>
+      <c r="S141" s="1">
+        <v>88</v>
+      </c>
+      <c r="T141" s="1">
+        <v>94</v>
+      </c>
+      <c r="U141" s="1">
+        <v>110</v>
+      </c>
       <c r="V141" s="1">
         <v>999</v>
       </c>
@@ -8990,28 +9022,234 @@
       <c r="X141" s="1"/>
     </row>
     <row r="142" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A142" s="1"/>
-      <c r="B142" s="1"/>
-      <c r="C142" s="1"/>
-      <c r="D142" s="1"/>
-      <c r="E142" s="1"/>
-      <c r="F142" s="1"/>
-      <c r="G142" s="1"/>
-      <c r="J142" s="1"/>
-      <c r="K142" s="1"/>
+      <c r="A142" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E142" s="4">
+        <v>95</v>
+      </c>
+      <c r="F142" s="4">
+        <v>99</v>
+      </c>
+      <c r="G142" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I142" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J142"/>
+      <c r="K142"/>
       <c r="L142" s="1"/>
-      <c r="M142" s="1"/>
       <c r="N142" s="1"/>
-      <c r="O142" s="1"/>
-      <c r="P142" s="1"/>
-      <c r="Q142" s="1"/>
-      <c r="R142" s="1"/>
-      <c r="S142" s="1"/>
-      <c r="T142" s="1"/>
-      <c r="U142" s="1"/>
-      <c r="V142" s="1"/>
+      <c r="O142" s="1">
+        <v>60</v>
+      </c>
+      <c r="P142" s="1">
+        <v>65</v>
+      </c>
+      <c r="Q142" s="1">
+        <v>71</v>
+      </c>
+      <c r="R142" s="1">
+        <v>79</v>
+      </c>
+      <c r="S142" s="1">
+        <v>88</v>
+      </c>
+      <c r="T142" s="1">
+        <v>94</v>
+      </c>
+      <c r="U142" s="1">
+        <v>110</v>
+      </c>
+      <c r="V142" s="1">
+        <v>999</v>
+      </c>
       <c r="W142" s="1"/>
       <c r="X142" s="1"/>
+    </row>
+    <row r="143" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E143" s="4">
+        <v>100</v>
+      </c>
+      <c r="F143" s="4">
+        <v>999</v>
+      </c>
+      <c r="G143" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J143"/>
+      <c r="K143"/>
+      <c r="L143" s="1"/>
+      <c r="N143" s="1"/>
+      <c r="O143" s="1">
+        <v>60</v>
+      </c>
+      <c r="P143" s="1">
+        <v>65</v>
+      </c>
+      <c r="Q143" s="1">
+        <v>71</v>
+      </c>
+      <c r="R143" s="1">
+        <v>79</v>
+      </c>
+      <c r="S143" s="1">
+        <v>88</v>
+      </c>
+      <c r="T143" s="1">
+        <v>94</v>
+      </c>
+      <c r="U143" s="1">
+        <v>110</v>
+      </c>
+      <c r="V143" s="1">
+        <v>999</v>
+      </c>
+      <c r="W143" s="1"/>
+      <c r="X143" s="1"/>
+    </row>
+    <row r="144" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E144" s="4">
+        <v>0</v>
+      </c>
+      <c r="F144" s="4">
+        <v>999</v>
+      </c>
+      <c r="G144" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H144" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J144" s="1"/>
+      <c r="K144" s="1"/>
+      <c r="L144" s="1"/>
+      <c r="N144" s="1"/>
+      <c r="O144" s="1"/>
+      <c r="P144" s="1"/>
+      <c r="Q144" s="1"/>
+      <c r="R144" s="1"/>
+      <c r="S144" s="1"/>
+      <c r="T144" s="1"/>
+      <c r="U144" s="1"/>
+      <c r="V144" s="1">
+        <v>999</v>
+      </c>
+      <c r="W144" s="1"/>
+      <c r="X144" s="1"/>
+    </row>
+    <row r="145" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E145" s="4">
+        <v>35</v>
+      </c>
+      <c r="F145" s="4">
+        <v>999</v>
+      </c>
+      <c r="G145" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H145" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I145" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J145" s="1"/>
+      <c r="K145" s="1"/>
+      <c r="L145" s="1"/>
+      <c r="N145" s="1"/>
+      <c r="O145" s="1"/>
+      <c r="P145" s="1"/>
+      <c r="Q145" s="1"/>
+      <c r="R145" s="1"/>
+      <c r="S145" s="1"/>
+      <c r="T145" s="1"/>
+      <c r="U145" s="1"/>
+      <c r="V145" s="1">
+        <v>999</v>
+      </c>
+      <c r="W145" s="1"/>
+      <c r="X145" s="1"/>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="1"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="J146" s="1"/>
+      <c r="K146" s="1"/>
+      <c r="L146" s="1"/>
+      <c r="M146" s="1"/>
+      <c r="N146" s="1"/>
+      <c r="O146" s="1"/>
+      <c r="P146" s="1"/>
+      <c r="Q146" s="1"/>
+      <c r="R146" s="1"/>
+      <c r="S146" s="1"/>
+      <c r="T146" s="1"/>
+      <c r="U146" s="1"/>
+      <c r="V146" s="1"/>
+      <c r="W146" s="1"/>
+      <c r="X146" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>